<commit_message>
isotope model version update
added several new graphs
some predictive modeling now implimented but not worknig well
added evaluation of model output
</commit_message>
<xml_diff>
--- a/file2.xlsx
+++ b/file2.xlsx
@@ -1,24 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanrh/Documents/GitHub/geochem_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32B9D67-9CBF-5147-93A5-DCFB21358CA4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163AB180-5A47-4F4F-B0C3-92A72846CCF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="28160" windowHeight="16720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="28160" windowHeight="16660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>A_o</t>
   </si>
@@ -447,7 +455,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -541,8 +549,8 @@
       <c r="E4" s="4">
         <v>-1.34226979279054</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>6</v>
+      <c r="F4" s="5">
+        <v>-2.5</v>
       </c>
       <c r="G4">
         <v>-2.4500000000000002</v>
@@ -598,8 +606,8 @@
       <c r="A7">
         <v>172800</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>6</v>
+      <c r="B7" s="5">
+        <v>3</v>
       </c>
       <c r="C7" s="4">
         <v>3.13781469253734</v>

</xml_diff>